<commit_message>
Rename Raspberry & Bar Bar Jinks
</commit_message>
<xml_diff>
--- a/SWGoH_Shard.xlsx
+++ b/SWGoH_Shard.xlsx
@@ -20,8 +20,8 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
     <customWorkbookView name="Selected Rows &amp; Columns" guid="{C889AC74-BC82-49E8-BA01-AB64462BFCF2}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
-    <customWorkbookView name="All Columns &amp; Rows" guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -314,9 +314,6 @@
     <t>&lt;https://swgoh.gg/u/berniewankensanders/&gt;</t>
   </si>
   <si>
-    <t>RΔsρberry</t>
-  </si>
-  <si>
     <t>USA, Oregon</t>
   </si>
   <si>
@@ -350,9 +347,6 @@
     <t>5/11</t>
   </si>
   <si>
-    <t>Bar Bar Jinks</t>
-  </si>
-  <si>
     <t>Guam</t>
   </si>
   <si>
@@ -396,6 +390,12 @@
   </si>
   <si>
     <t>:flag_jp:</t>
+  </si>
+  <si>
+    <t>Obi Wankin Obi</t>
+  </si>
+  <si>
+    <t>Raspywalker</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,29 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -833,15 +855,19 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -850,6 +876,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -858,27 +885,23 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -891,115 +914,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1044,166 +965,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF305496"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF920000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1648,10 +1409,10 @@
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M1" s="3" t="str">
         <f>H3</f>
@@ -1702,2203 +1463,2203 @@
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="7">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="50">
-        <v>25</v>
-      </c>
-      <c r="D2" s="50">
-        <v>1</v>
-      </c>
-      <c r="E2" s="51" t="s">
+      <c r="G2" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="H2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="52" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2" s="53">
+      <c r="I2" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="31">
+      <c r="K2" s="12"/>
+      <c r="L2" s="13">
         <f>$I2+Sheet2!B$1/24</f>
         <v>0.75</v>
       </c>
-      <c r="M2" s="31">
+      <c r="M2" s="13">
         <f>$I2+Sheet2!B$2/24</f>
         <v>0.70833333333333326</v>
       </c>
-      <c r="N2" s="31">
+      <c r="N2" s="13">
         <f>$I2+Sheet2!B$3/24</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="O2" s="31">
+      <c r="O2" s="13">
         <f>$I2+Sheet2!B$4/24</f>
         <v>0.45833333333333331</v>
       </c>
-      <c r="P2" s="31">
+      <c r="P2" s="13">
         <f>$I2+Sheet2!B$5/24</f>
         <v>0.45833333333333331</v>
       </c>
-      <c r="Q2" s="31">
+      <c r="Q2" s="13">
         <f>$I2+Sheet2!B$6/24</f>
         <v>0.45833333333333331</v>
       </c>
-      <c r="R2" s="31">
+      <c r="R2" s="13">
         <f>$I2+Sheet2!B$7/24</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="S2" s="31">
+      <c r="S2" s="13">
         <f>$I2+Sheet2!B$8/24</f>
         <v>0.375</v>
       </c>
-      <c r="T2" s="31">
+      <c r="T2" s="13">
         <f>$I2+Sheet2!B$9/24</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="U2" s="31">
+      <c r="U2" s="13">
         <f>$I2+Sheet2!B$10/24</f>
         <v>0.12499999999999997</v>
       </c>
-      <c r="V2" s="31">
+      <c r="V2" s="13">
         <f>$I2+Sheet2!B$11/24</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="W2" s="31">
+      <c r="W2" s="13">
         <f>$I2+Sheet2!B$12/24</f>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="33">
+      <c r="B3" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="15">
         <v>27</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="15">
         <v>2</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" s="36">
+      <c r="G3" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="18">
         <v>0.375</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="36">
+      <c r="K3" s="20"/>
+      <c r="L3" s="18">
         <f>$I3+Sheet2!B$1/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="M3" s="36">
+      <c r="M3" s="18">
         <f>$I3+Sheet2!B$2/24</f>
         <v>0.75</v>
       </c>
-      <c r="N3" s="36">
+      <c r="N3" s="18">
         <f>$I3+Sheet2!B$3/24</f>
         <v>0.70833333333333326</v>
       </c>
-      <c r="O3" s="36">
+      <c r="O3" s="18">
         <f>$I3+Sheet2!B$4/24</f>
         <v>0.5</v>
       </c>
-      <c r="P3" s="36">
+      <c r="P3" s="18">
         <f>$I3+Sheet2!B$5/24</f>
         <v>0.5</v>
       </c>
-      <c r="Q3" s="36">
+      <c r="Q3" s="18">
         <f>$I3+Sheet2!B$6/24</f>
         <v>0.5</v>
       </c>
-      <c r="R3" s="36">
+      <c r="R3" s="18">
         <f>$I3+Sheet2!B$7/24</f>
         <v>0.45833333333333331</v>
       </c>
-      <c r="S3" s="36">
+      <c r="S3" s="18">
         <f>$I3+Sheet2!B$8/24</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="T3" s="36">
+      <c r="T3" s="18">
         <f>$I3+Sheet2!B$9/24</f>
         <v>0.20833333333333334</v>
       </c>
-      <c r="U3" s="36">
+      <c r="U3" s="18">
         <f>$I3+Sheet2!B$10/24</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="V3" s="36">
+      <c r="V3" s="18">
         <f>$I3+Sheet2!B$11/24</f>
         <v>0.125</v>
       </c>
-      <c r="W3" s="36">
+      <c r="W3" s="18">
         <f>$I3+Sheet2!B$12/24</f>
         <v>8.3333333333333315E-2</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="23">
         <v>15</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="24">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="11" t="str">
+      <c r="H4" s="25" t="str">
         <f>Sheet2!$A$3</f>
         <v>CST</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="26">
         <v>0.41666666666666669</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="12">
+      <c r="K4" s="20"/>
+      <c r="L4" s="26">
         <f>$I4+Sheet2!B$1/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="26">
         <f>$I4+Sheet2!B$2/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="26">
         <f>$I4+Sheet2!B$3/24</f>
         <v>0.75</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="26">
         <f>$I4+Sheet2!B$4/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="26">
         <f>$I4+Sheet2!B$5/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="26">
         <f>$I4+Sheet2!B$6/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="R4" s="12">
+      <c r="R4" s="26">
         <f>$I4+Sheet2!B$7/24</f>
         <v>0.5</v>
       </c>
-      <c r="S4" s="12">
+      <c r="S4" s="26">
         <f>$I4+Sheet2!B$8/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="T4" s="12">
+      <c r="T4" s="26">
         <f>$I4+Sheet2!B$9/24</f>
         <v>0.25</v>
       </c>
-      <c r="U4" s="12">
+      <c r="U4" s="26">
         <f>$I4+Sheet2!B$10/24</f>
         <v>0.20833333333333334</v>
       </c>
-      <c r="V4" s="12">
+      <c r="V4" s="26">
         <f>$I4+Sheet2!B$11/24</f>
         <v>0.16666666666666669</v>
       </c>
-      <c r="W4" s="12">
+      <c r="W4" s="26">
         <f>$I4+Sheet2!B$12/24</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="58">
+      <c r="C5" s="29">
         <v>11</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="29">
         <v>4</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="59" t="s">
+      <c r="F5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="60" t="str">
+      <c r="H5" s="31" t="str">
         <f>Sheet2!$A$4</f>
         <v>MSK</v>
       </c>
-      <c r="I5" s="61">
+      <c r="I5" s="32">
         <v>0.625</v>
       </c>
-      <c r="J5" s="62" t="s">
+      <c r="J5" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="L5" s="64">
+      <c r="K5" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="35">
         <f>$I5+Sheet2!B$1/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="M5" s="61">
+      <c r="M5" s="32">
         <f>$I5+Sheet2!B$2/24</f>
         <v>1</v>
       </c>
-      <c r="N5" s="61">
+      <c r="N5" s="32">
         <f>$I5+Sheet2!B$3/24</f>
         <v>0.95833333333333326</v>
       </c>
-      <c r="O5" s="61">
+      <c r="O5" s="32">
         <f>$I5+Sheet2!B$4/24</f>
         <v>0.75</v>
       </c>
-      <c r="P5" s="61">
+      <c r="P5" s="32">
         <f>$I5+Sheet2!B$5/24</f>
         <v>0.75</v>
       </c>
-      <c r="Q5" s="61">
+      <c r="Q5" s="32">
         <f>$I5+Sheet2!B$6/24</f>
         <v>0.75</v>
       </c>
-      <c r="R5" s="61">
+      <c r="R5" s="32">
         <f>$I5+Sheet2!B$7/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="S5" s="61">
+      <c r="S5" s="32">
         <f>$I5+Sheet2!B$8/24</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="T5" s="61">
+      <c r="T5" s="32">
         <f>$I5+Sheet2!B$9/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="U5" s="61">
+      <c r="U5" s="32">
         <f>$I5+Sheet2!B$10/24</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="V5" s="61">
+      <c r="V5" s="32">
         <f>$I5+Sheet2!B$11/24</f>
         <v>0.375</v>
       </c>
-      <c r="W5" s="61">
+      <c r="W5" s="32">
         <f>$I5+Sheet2!B$12/24</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="38">
         <v>12</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="38">
         <v>5</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="21" t="str">
+      <c r="H6" s="41" t="str">
         <f>Sheet2!$A$4</f>
         <v>MSK</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="42">
         <v>0.625</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="L6" s="24">
+      <c r="K6" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L6" s="45">
         <f>$I6+Sheet2!B$1/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="42">
         <f>$I6+Sheet2!B$2/24</f>
         <v>1</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="42">
         <f>$I6+Sheet2!B$3/24</f>
         <v>0.95833333333333326</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="42">
         <f>$I6+Sheet2!B$4/24</f>
         <v>0.75</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="42">
         <f>$I6+Sheet2!B$5/24</f>
         <v>0.75</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="42">
         <f>$I6+Sheet2!B$6/24</f>
         <v>0.75</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="42">
         <f>$I6+Sheet2!B$7/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="42">
         <f>$I6+Sheet2!B$8/24</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="T6" s="6">
+      <c r="T6" s="42">
         <f>$I6+Sheet2!B$9/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="42">
         <f>$I6+Sheet2!B$10/24</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="42">
         <f>$I6+Sheet2!B$11/24</f>
         <v>0.375</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W6" s="42">
         <f>$I6+Sheet2!B$12/24</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="38">
         <v>14</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="38">
         <v>6</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="21" t="str">
+      <c r="H7" s="41" t="str">
         <f>Sheet2!$A$4</f>
         <v>MSK</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="42">
         <v>0.625</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" s="31">
+      <c r="K7" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="13">
         <f>$I7+Sheet2!B$1/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="42">
         <f>$I7+Sheet2!B$2/24</f>
         <v>1</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="42">
         <f>$I7+Sheet2!B$3/24</f>
         <v>0.95833333333333326</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="42">
         <f>$I7+Sheet2!B$4/24</f>
         <v>0.75</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="42">
         <f>$I7+Sheet2!B$5/24</f>
         <v>0.75</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="42">
         <f>$I7+Sheet2!B$6/24</f>
         <v>0.75</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="42">
         <f>$I7+Sheet2!B$7/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="42">
         <f>$I7+Sheet2!B$8/24</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="42">
         <f>$I7+Sheet2!B$9/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="42">
         <f>$I7+Sheet2!B$10/24</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="V7" s="6">
+      <c r="V7" s="42">
         <f>$I7+Sheet2!B$11/24</f>
         <v>0.375</v>
       </c>
-      <c r="W7" s="6">
+      <c r="W7" s="42">
         <f>$I7+Sheet2!B$12/24</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="38">
         <v>21</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="38">
         <v>7</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="21" t="str">
+      <c r="H8" s="41" t="str">
         <f>Sheet2!$A$4</f>
         <v>MSK</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="42">
         <v>0.625</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="L8" s="24">
+      <c r="K8" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="45">
         <f>$I8+Sheet2!B$1/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="42">
         <f>$I8+Sheet2!B$2/24</f>
         <v>1</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="42">
         <f>$I8+Sheet2!B$3/24</f>
         <v>0.95833333333333326</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="42">
         <f>$I8+Sheet2!B$4/24</f>
         <v>0.75</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="42">
         <f>$I8+Sheet2!B$5/24</f>
         <v>0.75</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="42">
         <f>$I8+Sheet2!B$6/24</f>
         <v>0.75</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="42">
         <f>$I8+Sheet2!B$7/24</f>
         <v>0.70833333333333337</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="42">
         <f>$I8+Sheet2!B$8/24</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="42">
         <f>$I8+Sheet2!B$9/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="U8" s="6">
+      <c r="U8" s="42">
         <f>$I8+Sheet2!B$10/24</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="V8" s="6">
+      <c r="V8" s="42">
         <f>$I8+Sheet2!B$11/24</f>
         <v>0.375</v>
       </c>
-      <c r="W8" s="6">
+      <c r="W8" s="42">
         <f>$I8+Sheet2!B$12/24</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="47" t="s">
+      <c r="A9" s="36"/>
+      <c r="B9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="15">
         <v>4</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="15">
         <v>8</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="56" t="str">
+      <c r="H9" s="17" t="str">
         <f>Sheet2!$A$5</f>
         <v>TRT</v>
       </c>
-      <c r="I9" s="36">
+      <c r="I9" s="18">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="L9" s="38">
+      <c r="K9" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="47">
         <f>$I9+Sheet2!B$1/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="M9" s="36">
+      <c r="M9" s="18">
         <f>$I9+Sheet2!B$2/24</f>
         <v>1.0416666666666665</v>
       </c>
-      <c r="N9" s="36">
+      <c r="N9" s="18">
         <f>$I9+Sheet2!B$3/24</f>
         <v>1</v>
       </c>
-      <c r="O9" s="36">
+      <c r="O9" s="18">
         <f>$I9+Sheet2!B$4/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="P9" s="36">
+      <c r="P9" s="18">
         <f>$I9+Sheet2!B$5/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="Q9" s="36">
+      <c r="Q9" s="18">
         <f>$I9+Sheet2!B$6/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="R9" s="36">
+      <c r="R9" s="18">
         <f>$I9+Sheet2!B$7/24</f>
         <v>0.75</v>
       </c>
-      <c r="S9" s="36">
+      <c r="S9" s="18">
         <f>$I9+Sheet2!B$8/24</f>
         <v>0.70833333333333326</v>
       </c>
-      <c r="T9" s="36">
+      <c r="T9" s="18">
         <f>$I9+Sheet2!B$9/24</f>
         <v>0.5</v>
       </c>
-      <c r="U9" s="36">
+      <c r="U9" s="18">
         <f>$I9+Sheet2!B$10/24</f>
         <v>0.45833333333333326</v>
       </c>
-      <c r="V9" s="36">
+      <c r="V9" s="18">
         <f>$I9+Sheet2!B$11/24</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="W9" s="36">
+      <c r="W9" s="18">
         <f>$I9+Sheet2!B$12/24</f>
         <v>0.37499999999999994</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="36"/>
+      <c r="B10" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="38">
         <v>7</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="38">
         <v>9</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="21" t="str">
+      <c r="H10" s="41" t="str">
         <f>Sheet2!$A$6</f>
         <v>EEST</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="42">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="L10" s="24">
+      <c r="K10" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="45">
         <f>$I10+Sheet2!B$1/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="42">
         <f>$I10+Sheet2!B$2/24</f>
         <v>1.0416666666666665</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="42">
         <f>$I10+Sheet2!B$3/24</f>
         <v>1</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="42">
         <f>$I10+Sheet2!B$4/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="42">
         <f>$I10+Sheet2!B$5/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="42">
         <f>$I10+Sheet2!B$6/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="42">
         <f>$I10+Sheet2!B$7/24</f>
         <v>0.75</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="42">
         <f>$I10+Sheet2!B$8/24</f>
         <v>0.70833333333333326</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T10" s="42">
         <f>$I10+Sheet2!B$9/24</f>
         <v>0.5</v>
       </c>
-      <c r="U10" s="6">
+      <c r="U10" s="42">
         <f>$I10+Sheet2!B$10/24</f>
         <v>0.45833333333333326</v>
       </c>
-      <c r="V10" s="6">
+      <c r="V10" s="42">
         <f>$I10+Sheet2!B$11/24</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="W10" s="6">
+      <c r="W10" s="42">
         <f>$I10+Sheet2!B$12/24</f>
         <v>0.37499999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="47" t="s">
+      <c r="A11" s="36"/>
+      <c r="B11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="15">
         <v>1</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="15">
         <v>10</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="35" t="str">
+      <c r="H11" s="50" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
-      <c r="I11" s="36">
+      <c r="I11" s="18">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J11" s="37" t="s">
+      <c r="J11" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="L11" s="38">
+      <c r="K11" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="L11" s="47">
         <f>$I11+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="M11" s="36">
+      <c r="M11" s="18">
         <f>$I11+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="18">
         <f>$I11+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="O11" s="36">
+      <c r="O11" s="18">
         <f>$I11+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P11" s="36">
+      <c r="P11" s="18">
         <f>$I11+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q11" s="36">
+      <c r="Q11" s="18">
         <f>$I11+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R11" s="36">
+      <c r="R11" s="18">
         <f>$I11+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="S11" s="36">
+      <c r="S11" s="18">
         <f>$I11+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="T11" s="36">
+      <c r="T11" s="18">
         <f>$I11+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="U11" s="36">
+      <c r="U11" s="18">
         <f>$I11+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="V11" s="36">
+      <c r="V11" s="18">
         <f>$I11+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="W11" s="36">
+      <c r="W11" s="18">
         <f>$I11+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="38">
         <v>2</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="38">
         <v>11</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="28" t="str">
+      <c r="H12" s="52" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="42">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" s="24">
+      <c r="K12" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="45">
         <f>$I12+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="42">
         <f>$I12+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="42">
         <f>$I12+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="42">
         <f>$I12+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="42">
         <f>$I12+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12" s="42">
         <f>$I12+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="42">
         <f>$I12+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="S12" s="6">
+      <c r="S12" s="42">
         <f>$I12+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="T12" s="6">
+      <c r="T12" s="42">
         <f>$I12+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="U12" s="6">
+      <c r="U12" s="42">
         <f>$I12+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="V12" s="6">
+      <c r="V12" s="42">
         <f>$I12+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="W12" s="6">
+      <c r="W12" s="42">
         <f>$I12+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="38">
         <v>5</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="38">
         <v>12</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="28" t="str">
+      <c r="H13" s="52" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="42">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="L13" s="31">
+      <c r="K13" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="L13" s="13">
         <f>$I13+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="42">
         <f>$I13+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="42">
         <f>$I13+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="42">
         <f>$I13+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="42">
         <f>$I13+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="42">
         <f>$I13+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="42">
         <f>$I13+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="42">
         <f>$I13+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="T13" s="6">
+      <c r="T13" s="42">
         <f>$I13+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="42">
         <f>$I13+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="V13" s="6">
+      <c r="V13" s="42">
         <f>$I13+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="W13" s="6">
+      <c r="W13" s="42">
         <f>$I13+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="38">
         <v>16</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="38">
         <v>13</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="28" t="str">
+      <c r="H14" s="52" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="42">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="L14" s="24">
+      <c r="K14" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" s="45">
         <f>$I14+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="42">
         <f>$I14+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="42">
         <f>$I14+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="42">
         <f>$I14+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="42">
         <f>$I14+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14" s="42">
         <f>$I14+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R14" s="42">
         <f>$I14+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="S14" s="6">
+      <c r="S14" s="42">
         <f>$I14+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="T14" s="6">
+      <c r="T14" s="42">
         <f>$I14+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="U14" s="6">
+      <c r="U14" s="42">
         <f>$I14+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="V14" s="6">
+      <c r="V14" s="42">
         <f>$I14+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="W14" s="6">
+      <c r="W14" s="42">
         <f>$I14+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="36"/>
+      <c r="B15" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="38">
         <v>19</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="38">
         <v>14</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="28" t="str">
+      <c r="H15" s="52" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="42">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="L15" s="31">
+      <c r="K15" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" s="13">
         <f>$I15+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="42">
         <f>$I15+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="N15" s="6">
+      <c r="N15" s="42">
         <f>$I15+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="42">
         <f>$I15+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="42">
         <f>$I15+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="Q15" s="42">
         <f>$I15+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R15" s="6">
+      <c r="R15" s="42">
         <f>$I15+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="42">
         <f>$I15+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="T15" s="6">
+      <c r="T15" s="42">
         <f>$I15+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="U15" s="6">
+      <c r="U15" s="42">
         <f>$I15+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="V15" s="6">
+      <c r="V15" s="42">
         <f>$I15+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="W15" s="6">
+      <c r="W15" s="42">
         <f>$I15+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="38">
         <v>20</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="38">
         <v>15</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="28" t="str">
+      <c r="H16" s="52" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="42">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="L16" s="24">
+      <c r="K16" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="L16" s="45">
         <f>$I16+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="42">
         <f>$I16+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="N16" s="6">
+      <c r="N16" s="42">
         <f>$I16+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="42">
         <f>$I16+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P16" s="6">
+      <c r="P16" s="42">
         <f>$I16+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="Q16" s="42">
         <f>$I16+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R16" s="6">
+      <c r="R16" s="42">
         <f>$I16+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="S16" s="6">
+      <c r="S16" s="42">
         <f>$I16+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="T16" s="6">
+      <c r="T16" s="42">
         <f>$I16+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="U16" s="6">
+      <c r="U16" s="42">
         <f>$I16+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="V16" s="6">
+      <c r="V16" s="42">
         <f>$I16+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="W16" s="6">
+      <c r="W16" s="42">
         <f>$I16+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="38">
         <v>24</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="38">
         <v>16</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="H17" s="28" t="str">
+      <c r="H17" s="52" t="str">
         <f>Sheet2!$A$7</f>
         <v>CEST</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="42">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="L17" s="31">
+      <c r="K17" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="L17" s="13">
         <f>$I17+Sheet2!B$1/24</f>
         <v>1.125</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="42">
         <f>$I17+Sheet2!B$2/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="N17" s="6">
+      <c r="N17" s="42">
         <f>$I17+Sheet2!B$3/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="42">
         <f>$I17+Sheet2!B$4/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="P17" s="6">
+      <c r="P17" s="42">
         <f>$I17+Sheet2!B$5/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="Q17" s="42">
         <f>$I17+Sheet2!B$6/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R17" s="42">
         <f>$I17+Sheet2!B$7/24</f>
         <v>0.79166666666666674</v>
       </c>
-      <c r="S17" s="6">
+      <c r="S17" s="42">
         <f>$I17+Sheet2!B$8/24</f>
         <v>0.75</v>
       </c>
-      <c r="T17" s="6">
+      <c r="T17" s="42">
         <f>$I17+Sheet2!B$9/24</f>
         <v>0.54166666666666674</v>
       </c>
-      <c r="U17" s="6">
+      <c r="U17" s="42">
         <f>$I17+Sheet2!B$10/24</f>
         <v>0.5</v>
       </c>
-      <c r="V17" s="6">
+      <c r="V17" s="42">
         <f>$I17+Sheet2!B$11/24</f>
         <v>0.45833333333333337</v>
       </c>
-      <c r="W17" s="6">
+      <c r="W17" s="42">
         <f>$I17+Sheet2!B$12/24</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="36"/>
+      <c r="B18" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="15">
         <v>22</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="16">
         <v>17</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G18" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="36">
+      <c r="I18" s="18">
         <v>0.75</v>
       </c>
-      <c r="J18" s="37" t="s">
+      <c r="J18" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="L18" s="48">
+      <c r="K18" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="L18" s="54">
         <f>$I18+Sheet2!B$1/24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="M18" s="36">
+      <c r="M18" s="18">
         <f>$I18+Sheet2!B$2/24</f>
         <v>1.125</v>
       </c>
-      <c r="N18" s="36">
+      <c r="N18" s="18">
         <f>$I18+Sheet2!B$3/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="O18" s="36">
+      <c r="O18" s="18">
         <f>$I18+Sheet2!B$4/24</f>
         <v>0.875</v>
       </c>
-      <c r="P18" s="36">
+      <c r="P18" s="18">
         <f>$I18+Sheet2!B$5/24</f>
         <v>0.875</v>
       </c>
-      <c r="Q18" s="36">
+      <c r="Q18" s="18">
         <f>$I18+Sheet2!B$6/24</f>
         <v>0.875</v>
       </c>
-      <c r="R18" s="36">
+      <c r="R18" s="18">
         <f>$I18+Sheet2!B$7/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="S18" s="36">
+      <c r="S18" s="18">
         <f>$I18+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="T18" s="36">
+      <c r="T18" s="18">
         <f>$I18+Sheet2!B$9/24</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="U18" s="36">
+      <c r="U18" s="18">
         <f>$I18+Sheet2!B$10/24</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="V18" s="36">
+      <c r="V18" s="18">
         <f>$I18+Sheet2!B$11/24</f>
         <v>0.5</v>
       </c>
-      <c r="W18" s="36">
+      <c r="W18" s="18">
         <f>$I18+Sheet2!B$12/24</f>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="40">
+      <c r="A19" s="55"/>
+      <c r="B19" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="57">
         <v>26</v>
       </c>
-      <c r="D19" s="41">
+      <c r="D19" s="58">
         <v>18</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" s="42" t="s">
+      <c r="G19" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43">
+      <c r="I19" s="60">
         <v>0.75</v>
       </c>
-      <c r="J19" s="44" t="s">
+      <c r="J19" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="L19" s="46">
+      <c r="K19" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="L19" s="63">
         <f>$I19+Sheet2!B$1/24</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="M19" s="43">
+      <c r="M19" s="60">
         <f>$I19+Sheet2!B$2/24</f>
         <v>1.125</v>
       </c>
-      <c r="N19" s="43">
+      <c r="N19" s="60">
         <f>$I19+Sheet2!B$3/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="O19" s="43">
+      <c r="O19" s="60">
         <f>$I19+Sheet2!B$4/24</f>
         <v>0.875</v>
       </c>
-      <c r="P19" s="43">
+      <c r="P19" s="60">
         <f>$I19+Sheet2!B$5/24</f>
         <v>0.875</v>
       </c>
-      <c r="Q19" s="43">
+      <c r="Q19" s="60">
         <f>$I19+Sheet2!B$6/24</f>
         <v>0.875</v>
       </c>
-      <c r="R19" s="43">
+      <c r="R19" s="60">
         <f>$I19+Sheet2!B$7/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="S19" s="43">
+      <c r="S19" s="60">
         <f>$I19+Sheet2!B$8/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="T19" s="43">
+      <c r="T19" s="60">
         <f>$I19+Sheet2!B$9/24</f>
         <v>0.58333333333333337</v>
       </c>
-      <c r="U19" s="43">
+      <c r="U19" s="60">
         <f>$I19+Sheet2!B$10/24</f>
         <v>0.54166666666666663</v>
       </c>
-      <c r="V19" s="43">
+      <c r="V19" s="60">
         <f>$I19+Sheet2!B$11/24</f>
         <v>0.5</v>
       </c>
-      <c r="W19" s="43">
+      <c r="W19" s="60">
         <f>$I19+Sheet2!B$12/24</f>
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="38">
         <v>3</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="38">
         <v>19</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="28" t="str">
+      <c r="H20" s="52" t="str">
         <f>Sheet2!$A$9</f>
         <v>EDT</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="42">
         <v>0.91666666666666696</v>
       </c>
-      <c r="J20" s="26" t="s">
+      <c r="J20" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="L20" s="31">
+      <c r="K20" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="L20" s="13">
         <f>$I20+Sheet2!B$1/24</f>
         <v>1.3333333333333337</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="42">
         <f>$I20+Sheet2!B$2/24</f>
         <v>1.291666666666667</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N20" s="42">
         <f>$I20+Sheet2!B$3/24</f>
         <v>1.2500000000000002</v>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="42">
         <f>$I20+Sheet2!B$4/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="P20" s="6">
+      <c r="P20" s="42">
         <f>$I20+Sheet2!B$5/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="Q20" s="6">
+      <c r="Q20" s="42">
         <f>$I20+Sheet2!B$6/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="R20" s="6">
+      <c r="R20" s="42">
         <f>$I20+Sheet2!B$7/24</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="S20" s="6">
+      <c r="S20" s="42">
         <f>$I20+Sheet2!B$8/24</f>
         <v>0.95833333333333359</v>
       </c>
-      <c r="T20" s="6">
+      <c r="T20" s="42">
         <f>$I20+Sheet2!B$9/24</f>
         <v>0.75000000000000033</v>
       </c>
-      <c r="U20" s="6">
+      <c r="U20" s="42">
         <f>$I20+Sheet2!B$10/24</f>
         <v>0.70833333333333359</v>
       </c>
-      <c r="V20" s="6">
+      <c r="V20" s="42">
         <f>$I20+Sheet2!B$11/24</f>
         <v>0.66666666666666696</v>
       </c>
-      <c r="W20" s="6">
+      <c r="W20" s="42">
         <f>$I20+Sheet2!B$12/24</f>
         <v>0.62500000000000022</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="18">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="38">
         <v>10</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="38">
         <v>20</v>
       </c>
-      <c r="E21" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="18" t="s">
+      <c r="E21" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="H21" s="28" t="str">
+      <c r="G21" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="52" t="str">
         <f>Sheet2!$A$9</f>
         <v>EDT</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="42">
         <v>0.91666666666666696</v>
       </c>
-      <c r="J21" s="26" t="s">
+      <c r="J21" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="L21" s="24">
+      <c r="K21" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" s="45">
         <f>$I21+Sheet2!B$1/24</f>
         <v>1.3333333333333337</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="42">
         <f>$I21+Sheet2!B$2/24</f>
         <v>1.291666666666667</v>
       </c>
-      <c r="N21" s="6">
+      <c r="N21" s="42">
         <f>$I21+Sheet2!B$3/24</f>
         <v>1.2500000000000002</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="42">
         <f>$I21+Sheet2!B$4/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="P21" s="6">
+      <c r="P21" s="42">
         <f>$I21+Sheet2!B$5/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="Q21" s="6">
+      <c r="Q21" s="42">
         <f>$I21+Sheet2!B$6/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="R21" s="6">
+      <c r="R21" s="42">
         <f>$I21+Sheet2!B$7/24</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="S21" s="6">
+      <c r="S21" s="42">
         <f>$I21+Sheet2!B$8/24</f>
         <v>0.95833333333333359</v>
       </c>
-      <c r="T21" s="6">
+      <c r="T21" s="42">
         <f>$I21+Sheet2!B$9/24</f>
         <v>0.75000000000000033</v>
       </c>
-      <c r="U21" s="6">
+      <c r="U21" s="42">
         <f>$I21+Sheet2!B$10/24</f>
         <v>0.70833333333333359</v>
       </c>
-      <c r="V21" s="6">
+      <c r="V21" s="42">
         <f>$I21+Sheet2!B$11/24</f>
         <v>0.66666666666666696</v>
       </c>
-      <c r="W21" s="6">
+      <c r="W21" s="42">
         <f>$I21+Sheet2!B$12/24</f>
         <v>0.62500000000000022</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17" t="s">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="38">
         <v>13</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="38">
         <v>21</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="28" t="str">
+      <c r="H22" s="52" t="str">
         <f>Sheet2!$A$9</f>
         <v>EDT</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="42">
         <v>0.91666666666666696</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="L22" s="24">
+      <c r="K22" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" s="45">
         <f>$I22+Sheet2!B$1/24</f>
         <v>1.3333333333333337</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="42">
         <f>$I22+Sheet2!B$2/24</f>
         <v>1.291666666666667</v>
       </c>
-      <c r="N22" s="6">
+      <c r="N22" s="42">
         <f>$I22+Sheet2!B$3/24</f>
         <v>1.2500000000000002</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="42">
         <f>$I22+Sheet2!B$4/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="P22" s="6">
+      <c r="P22" s="42">
         <f>$I22+Sheet2!B$5/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="Q22" s="6">
+      <c r="Q22" s="42">
         <f>$I22+Sheet2!B$6/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="R22" s="6">
+      <c r="R22" s="42">
         <f>$I22+Sheet2!B$7/24</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="S22" s="6">
+      <c r="S22" s="42">
         <f>$I22+Sheet2!B$8/24</f>
         <v>0.95833333333333359</v>
       </c>
-      <c r="T22" s="6">
+      <c r="T22" s="42">
         <f>$I22+Sheet2!B$9/24</f>
         <v>0.75000000000000033</v>
       </c>
-      <c r="U22" s="6">
+      <c r="U22" s="42">
         <f>$I22+Sheet2!B$10/24</f>
         <v>0.70833333333333359</v>
       </c>
-      <c r="V22" s="6">
+      <c r="V22" s="42">
         <f>$I22+Sheet2!B$11/24</f>
         <v>0.66666666666666696</v>
       </c>
-      <c r="W22" s="6">
+      <c r="W22" s="42">
         <f>$I22+Sheet2!B$12/24</f>
         <v>0.62500000000000022</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17" t="s">
+      <c r="A23" s="36"/>
+      <c r="B23" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="38">
         <v>18</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="38">
         <v>22</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="G23" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="28" t="str">
+      <c r="H23" s="52" t="str">
         <f>Sheet2!$A$9</f>
         <v>EDT</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="42">
         <v>0.91666666666666696</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="L23" s="31">
+      <c r="K23" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" s="13">
         <f>$I23+Sheet2!B$1/24</f>
         <v>1.3333333333333337</v>
       </c>
-      <c r="M23" s="6">
+      <c r="M23" s="42">
         <f>$I23+Sheet2!B$2/24</f>
         <v>1.291666666666667</v>
       </c>
-      <c r="N23" s="6">
+      <c r="N23" s="42">
         <f>$I23+Sheet2!B$3/24</f>
         <v>1.2500000000000002</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="42">
         <f>$I23+Sheet2!B$4/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="P23" s="6">
+      <c r="P23" s="42">
         <f>$I23+Sheet2!B$5/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="Q23" s="6">
+      <c r="Q23" s="42">
         <f>$I23+Sheet2!B$6/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="R23" s="6">
+      <c r="R23" s="42">
         <f>$I23+Sheet2!B$7/24</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="S23" s="6">
+      <c r="S23" s="42">
         <f>$I23+Sheet2!B$8/24</f>
         <v>0.95833333333333359</v>
       </c>
-      <c r="T23" s="6">
+      <c r="T23" s="42">
         <f>$I23+Sheet2!B$9/24</f>
         <v>0.75000000000000033</v>
       </c>
-      <c r="U23" s="6">
+      <c r="U23" s="42">
         <f>$I23+Sheet2!B$10/24</f>
         <v>0.70833333333333359</v>
       </c>
-      <c r="V23" s="6">
+      <c r="V23" s="42">
         <f>$I23+Sheet2!B$11/24</f>
         <v>0.66666666666666696</v>
       </c>
-      <c r="W23" s="6">
+      <c r="W23" s="42">
         <f>$I23+Sheet2!B$12/24</f>
         <v>0.62500000000000022</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="36"/>
+      <c r="B24" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="33">
+      <c r="C24" s="15">
         <v>6</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="16">
         <v>23</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="35" t="s">
+      <c r="G24" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="H24" s="35" t="str">
+      <c r="H24" s="50" t="str">
         <f>Sheet2!$A$9</f>
         <v>EDT</v>
       </c>
-      <c r="I24" s="36">
+      <c r="I24" s="18">
         <v>0.95833333333333359</v>
       </c>
-      <c r="J24" s="37" t="s">
+      <c r="J24" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="L24" s="48">
+      <c r="K24" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="L24" s="54">
         <f>$I24+Sheet2!B$1/24</f>
         <v>1.3750000000000002</v>
       </c>
-      <c r="M24" s="36">
+      <c r="M24" s="18">
         <f>$I24+Sheet2!B$2/24</f>
         <v>1.3333333333333335</v>
       </c>
-      <c r="N24" s="36">
+      <c r="N24" s="18">
         <f>$I24+Sheet2!B$3/24</f>
         <v>1.291666666666667</v>
       </c>
-      <c r="O24" s="36">
+      <c r="O24" s="18">
         <f>$I24+Sheet2!B$4/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="P24" s="36">
+      <c r="P24" s="18">
         <f>$I24+Sheet2!B$5/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="Q24" s="36">
+      <c r="Q24" s="18">
         <f>$I24+Sheet2!B$6/24</f>
         <v>1.0833333333333335</v>
       </c>
-      <c r="R24" s="36">
+      <c r="R24" s="18">
         <f>$I24+Sheet2!B$7/24</f>
         <v>1.041666666666667</v>
       </c>
-      <c r="S24" s="36">
+      <c r="S24" s="18">
         <f>$I24+Sheet2!B$8/24</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="T24" s="36">
+      <c r="T24" s="18">
         <f>$I24+Sheet2!B$9/24</f>
         <v>0.79166666666666696</v>
       </c>
-      <c r="U24" s="36">
+      <c r="U24" s="18">
         <f>$I24+Sheet2!B$10/24</f>
         <v>0.75000000000000022</v>
       </c>
-      <c r="V24" s="36">
+      <c r="V24" s="18">
         <f>$I24+Sheet2!B$11/24</f>
         <v>0.70833333333333359</v>
       </c>
-      <c r="W24" s="36">
+      <c r="W24" s="18">
         <f>$I24+Sheet2!B$12/24</f>
         <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17" t="s">
+      <c r="A25" s="36"/>
+      <c r="B25" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="38">
         <v>8</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="38">
         <v>24</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="G25" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="28" t="str">
+      <c r="H25" s="52" t="str">
         <f>Sheet2!$A$10</f>
         <v>CDT</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="42">
         <v>0.95833333333333304</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="L25" s="31">
+      <c r="K25" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="L25" s="13">
         <f>$I25+Sheet2!B$1/24</f>
         <v>1.3749999999999998</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M25" s="42">
         <f>$I25+Sheet2!B$2/24</f>
         <v>1.333333333333333</v>
       </c>
-      <c r="N25" s="6">
+      <c r="N25" s="42">
         <f>$I25+Sheet2!B$3/24</f>
         <v>1.2916666666666663</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="42">
         <f>$I25+Sheet2!B$4/24</f>
         <v>1.083333333333333</v>
       </c>
-      <c r="P25" s="6">
+      <c r="P25" s="42">
         <f>$I25+Sheet2!B$5/24</f>
         <v>1.083333333333333</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="Q25" s="42">
         <f>$I25+Sheet2!B$6/24</f>
         <v>1.083333333333333</v>
       </c>
-      <c r="R25" s="6">
+      <c r="R25" s="42">
         <f>$I25+Sheet2!B$7/24</f>
         <v>1.0416666666666663</v>
       </c>
-      <c r="S25" s="6">
+      <c r="S25" s="42">
         <f>$I25+Sheet2!B$8/24</f>
         <v>0.99999999999999967</v>
       </c>
-      <c r="T25" s="6">
+      <c r="T25" s="42">
         <f>$I25+Sheet2!B$9/24</f>
         <v>0.79166666666666641</v>
       </c>
-      <c r="U25" s="6">
+      <c r="U25" s="42">
         <f>$I25+Sheet2!B$10/24</f>
         <v>0.74999999999999967</v>
       </c>
-      <c r="V25" s="6">
+      <c r="V25" s="42">
         <f>$I25+Sheet2!B$11/24</f>
         <v>0.70833333333333304</v>
       </c>
-      <c r="W25" s="6">
+      <c r="W25" s="42">
         <f>$I25+Sheet2!B$12/24</f>
         <v>0.6666666666666663</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17" t="s">
+      <c r="A26" s="36"/>
+      <c r="B26" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="38">
         <v>23</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="38">
         <v>25</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G26" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="28" t="str">
+      <c r="H26" s="52" t="str">
         <f>Sheet2!$A$10</f>
         <v>CDT</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="42">
         <v>0.95833333333333304</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="L26" s="24">
+      <c r="K26" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="L26" s="45">
         <f>$I26+Sheet2!B$1/24</f>
         <v>1.3749999999999998</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M26" s="42">
         <f>$I26+Sheet2!B$2/24</f>
         <v>1.333333333333333</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N26" s="42">
         <f>$I26+Sheet2!B$3/24</f>
         <v>1.2916666666666663</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="42">
         <f>$I26+Sheet2!B$4/24</f>
         <v>1.083333333333333</v>
       </c>
-      <c r="P26" s="6">
+      <c r="P26" s="42">
         <f>$I26+Sheet2!B$5/24</f>
         <v>1.083333333333333</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="Q26" s="42">
         <f>$I26+Sheet2!B$6/24</f>
         <v>1.083333333333333</v>
       </c>
-      <c r="R26" s="6">
+      <c r="R26" s="42">
         <f>$I26+Sheet2!B$7/24</f>
         <v>1.0416666666666663</v>
       </c>
-      <c r="S26" s="6">
+      <c r="S26" s="42">
         <f>$I26+Sheet2!B$8/24</f>
         <v>0.99999999999999967</v>
       </c>
-      <c r="T26" s="6">
+      <c r="T26" s="42">
         <f>$I26+Sheet2!B$9/24</f>
         <v>0.79166666666666641</v>
       </c>
-      <c r="U26" s="6">
+      <c r="U26" s="42">
         <f>$I26+Sheet2!B$10/24</f>
         <v>0.74999999999999967</v>
       </c>
-      <c r="V26" s="6">
+      <c r="V26" s="42">
         <f>$I26+Sheet2!B$11/24</f>
         <v>0.70833333333333304</v>
       </c>
-      <c r="W26" s="6">
+      <c r="W26" s="42">
         <f>$I26+Sheet2!B$12/24</f>
         <v>0.6666666666666663</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="32" t="s">
+      <c r="A27" s="36"/>
+      <c r="B27" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="15">
         <v>17</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="15">
         <v>26</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="35" t="s">
+      <c r="G27" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="36">
+      <c r="I27" s="18">
         <v>1</v>
       </c>
-      <c r="J27" s="37" t="s">
+      <c r="J27" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="38">
+      <c r="K27" s="20"/>
+      <c r="L27" s="47">
         <f>$I27+Sheet2!B$1/24</f>
         <v>1.4166666666666667</v>
       </c>
-      <c r="M27" s="36">
+      <c r="M27" s="18">
         <f>$I27+Sheet2!B$2/24</f>
         <v>1.375</v>
       </c>
-      <c r="N27" s="36">
+      <c r="N27" s="18">
         <f>$I27+Sheet2!B$3/24</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="O27" s="36">
+      <c r="O27" s="18">
         <f>$I27+Sheet2!B$4/24</f>
         <v>1.125</v>
       </c>
-      <c r="P27" s="36">
+      <c r="P27" s="18">
         <f>$I27+Sheet2!B$5/24</f>
         <v>1.125</v>
       </c>
-      <c r="Q27" s="36">
+      <c r="Q27" s="18">
         <f>$I27+Sheet2!B$6/24</f>
         <v>1.125</v>
       </c>
-      <c r="R27" s="36">
+      <c r="R27" s="18">
         <f>$I27+Sheet2!B$7/24</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="S27" s="36">
+      <c r="S27" s="18">
         <f>$I27+Sheet2!B$8/24</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="T27" s="36">
+      <c r="T27" s="18">
         <f>$I27+Sheet2!B$9/24</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="U27" s="36">
+      <c r="U27" s="18">
         <f>$I27+Sheet2!B$10/24</f>
         <v>0.79166666666666663</v>
       </c>
-      <c r="V27" s="36">
+      <c r="V27" s="18">
         <f>$I27+Sheet2!B$11/24</f>
         <v>0.75</v>
       </c>
-      <c r="W27" s="36">
+      <c r="W27" s="18">
         <f>$I27+Sheet2!B$12/24</f>
         <v>0.70833333333333326</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="36"/>
+      <c r="B28" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="16">
+        <v>9</v>
+      </c>
+      <c r="D28" s="16">
+        <v>27</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C28" s="34">
-        <v>9</v>
-      </c>
-      <c r="D28" s="34">
-        <v>27</v>
-      </c>
-      <c r="E28" s="34" t="s">
+      <c r="F28" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="H28" s="28" t="str">
+      <c r="H28" s="52" t="str">
         <f>Sheet2!$A$12</f>
         <v>PDT</v>
       </c>
-      <c r="I28" s="36">
+      <c r="I28" s="18">
         <v>1.041666666666667</v>
       </c>
-      <c r="J28" s="37" t="s">
+      <c r="J28" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="14"/>
-      <c r="L28" s="48">
+      <c r="K28" s="20"/>
+      <c r="L28" s="54">
         <f>$I28+Sheet2!B$1/24</f>
         <v>1.4583333333333337</v>
       </c>
-      <c r="M28" s="36">
+      <c r="M28" s="18">
         <f>$I28+Sheet2!B$2/24</f>
         <v>1.416666666666667</v>
       </c>
-      <c r="N28" s="36">
+      <c r="N28" s="18">
         <f>$I28+Sheet2!B$3/24</f>
         <v>1.3750000000000002</v>
       </c>
-      <c r="O28" s="36">
+      <c r="O28" s="18">
         <f>$I28+Sheet2!B$4/24</f>
         <v>1.166666666666667</v>
       </c>
-      <c r="P28" s="36">
+      <c r="P28" s="18">
         <f>$I28+Sheet2!B$5/24</f>
         <v>1.166666666666667</v>
       </c>
-      <c r="Q28" s="36">
+      <c r="Q28" s="18">
         <f>$I28+Sheet2!B$6/24</f>
         <v>1.166666666666667</v>
       </c>
-      <c r="R28" s="36">
+      <c r="R28" s="18">
         <f>$I28+Sheet2!B$7/24</f>
         <v>1.1250000000000002</v>
       </c>
-      <c r="S28" s="36">
+      <c r="S28" s="18">
         <f>$I28+Sheet2!B$8/24</f>
         <v>1.0833333333333337</v>
       </c>
-      <c r="T28" s="36">
+      <c r="T28" s="18">
         <f>$I28+Sheet2!B$9/24</f>
         <v>0.87500000000000033</v>
       </c>
-      <c r="U28" s="36">
+      <c r="U28" s="18">
         <f>$I28+Sheet2!B$10/24</f>
         <v>0.83333333333333359</v>
       </c>
-      <c r="V28" s="36">
+      <c r="V28" s="18">
         <f>$I28+Sheet2!B$11/24</f>
         <v>0.79166666666666696</v>
       </c>
-      <c r="W28" s="36">
+      <c r="W28" s="18">
         <f>$I28+Sheet2!B$12/24</f>
         <v>0.75000000000000022</v>
       </c>
@@ -3908,10 +3669,10 @@
     <sortCondition ref="D2:D28"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{C889AC74-BC82-49E8-BA01-AB64462BFCF2}" hiddenColumns="1">
+    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{5D2AD3E2-CA0C-430D-85FE-AC4E745B5F2D}">
+    <customSheetView guid="{C889AC74-BC82-49E8-BA01-AB64462BFCF2}" hiddenColumns="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -3966,32 +3727,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:W28">
-    <cfRule type="expression" dxfId="0" priority="23">
+    <cfRule type="expression" dxfId="5" priority="23">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>M$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>M$1=$H18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>M$1=$H3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>L$1=$I2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>L$1=$H3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4017,24 +3778,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1">
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4045,7 +3806,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4056,7 +3817,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -4068,7 +3829,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -4085,7 +3846,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4101,7 +3862,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4117,7 +3878,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4133,7 +3894,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4149,7 +3910,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -4165,7 +3926,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,7 +3942,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>